<commit_message>
Tabela mediadaores por prof regente
</commit_message>
<xml_diff>
--- a/databases/parametros_turma.xlsx
+++ b/databases/parametros_turma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabalho\Anima\OneDrive - Administrativo - Ânima Educação\Projetos\Novo Modelo Acadêmico\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AFD1E4-47F4-4357-A2BD-7112FF3297E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87BF2B6-6753-45A9-BF37-BE60DBC8F150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2254,21 +2254,35 @@
   <autoFilter ref="A1:F202" xr:uid="{8EEE6562-8047-4AB2-AF29-4AA274593DC1}">
     <filterColumn colId="0">
       <filters>
-        <filter val="EAD 10.10"/>
         <filter val="Semi Presencial 30.20 Bacharelado"/>
-        <filter val="Semi Presencial 30.20 Licenciatura"/>
-        <filter val="Semi Presencial 40.20 Bacharelado"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="UC (10)"/>
+        <filter val="UC (1-3)"/>
+        <filter val="UC (1-5)"/>
+        <filter val="UC (1-6)"/>
+        <filter val="UC (4-8)"/>
+        <filter val="UC (6-10)"/>
+        <filter val="UC (6-8)"/>
+        <filter val="UC (7-8)"/>
+        <filter val="UC (7-9)"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="CH Semanal"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
       <filters>
-        <filter val="Mediador Assíncrono"/>
         <filter val="Mediador Online"/>
         <filter val="Mediador Presencial"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F163">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:F161">
     <sortCondition ref="A1:A202"/>
   </sortState>
   <tableColumns count="6">
@@ -2564,7 +2578,7 @@
   <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F17" sqref="A17:F19"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2620,7 +2634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2680,7 +2694,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2740,7 +2754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2900,7 +2914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2920,7 +2934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2940,7 +2954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -3080,7 +3094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3100,7 +3114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3120,7 +3134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -3860,7 +3874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -3880,7 +3894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" hidden="1">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -3900,7 +3914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -3940,7 +3954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" hidden="1">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -3960,7 +3974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" hidden="1">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -4000,7 +4014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -4020,7 +4034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -4040,7 +4054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -4060,7 +4074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -4160,7 +4174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" t="s">
         <v>20</v>
       </c>
@@ -4180,7 +4194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -4640,7 +4654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" hidden="1">
       <c r="A104" t="s">
         <v>23</v>
       </c>
@@ -4660,7 +4674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" hidden="1">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -4680,7 +4694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" hidden="1">
       <c r="A106" t="s">
         <v>23</v>
       </c>
@@ -4820,7 +4834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" hidden="1">
       <c r="A113" t="s">
         <v>23</v>
       </c>
@@ -4840,7 +4854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" hidden="1">
       <c r="A114" t="s">
         <v>23</v>
       </c>
@@ -4860,7 +4874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" hidden="1">
       <c r="A115" t="s">
         <v>23</v>
       </c>
@@ -4940,7 +4954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" hidden="1">
       <c r="A119" t="s">
         <v>23</v>
       </c>
@@ -4960,7 +4974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120" t="s">
         <v>23</v>
       </c>
@@ -4980,7 +4994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" hidden="1">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -5240,7 +5254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" hidden="1">
       <c r="A134" t="s">
         <v>24</v>
       </c>
@@ -5260,7 +5274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" hidden="1">
       <c r="A135" t="s">
         <v>24</v>
       </c>
@@ -5280,7 +5294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" hidden="1">
       <c r="A136" t="s">
         <v>24</v>
       </c>
@@ -5360,7 +5374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" hidden="1">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -5380,7 +5394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" hidden="1">
       <c r="A141" t="s">
         <v>24</v>
       </c>
@@ -5400,7 +5414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" hidden="1">
       <c r="A142" t="s">
         <v>24</v>
       </c>
@@ -5420,7 +5434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" hidden="1">
       <c r="A143" t="s">
         <v>24</v>
       </c>
@@ -5440,7 +5454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" hidden="1">
       <c r="A144" t="s">
         <v>24</v>
       </c>
@@ -5460,7 +5474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" hidden="1">
       <c r="A145" t="s">
         <v>24</v>
       </c>
@@ -5480,7 +5494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" hidden="1">
       <c r="A146" t="s">
         <v>24</v>
       </c>
@@ -5500,7 +5514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" hidden="1">
       <c r="A147" t="s">
         <v>24</v>
       </c>
@@ -5520,7 +5534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" hidden="1">
       <c r="A148" t="s">
         <v>24</v>
       </c>
@@ -5600,7 +5614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" hidden="1">
       <c r="A152" t="s">
         <v>24</v>
       </c>
@@ -5620,7 +5634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" hidden="1">
       <c r="A153" t="s">
         <v>24</v>
       </c>
@@ -5640,7 +5654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" hidden="1">
       <c r="A154" t="s">
         <v>24</v>
       </c>
@@ -5660,7 +5674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" hidden="1">
       <c r="A155" t="s">
         <v>24</v>
       </c>
@@ -5680,7 +5694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" hidden="1">
       <c r="A156" t="s">
         <v>24</v>
       </c>
@@ -5700,7 +5714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" hidden="1">
       <c r="A157" t="s">
         <v>24</v>
       </c>
@@ -5780,7 +5794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" hidden="1">
       <c r="A161" t="s">
         <v>24</v>
       </c>
@@ -5800,7 +5814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" hidden="1">
       <c r="A162" t="s">
         <v>24</v>
       </c>
@@ -5820,7 +5834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" hidden="1">
       <c r="A163" t="s">
         <v>24</v>
       </c>

</xml_diff>